<commit_message>
add email address for users selection
</commit_message>
<xml_diff>
--- a/cmu/SurePark/SurePark_Database.xlsx
+++ b/cmu/SurePark/SurePark_Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23715" windowHeight="9180" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="23715" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="USERS" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -429,6 +429,22 @@
   </si>
   <si>
     <t>단위는 달러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{userEmail:'gildong@lge.com'}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -597,8 +613,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="B2:F7" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="B2:F7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="B2:F8" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="B2:F8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="name" dataDxfId="9"/>
     <tableColumn id="2" name="type" dataDxfId="8"/>
@@ -925,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1016,15 +1032,29 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1266,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add displayName for users db
</commit_message>
<xml_diff>
--- a/cmu/SurePark/SurePark_Database.xlsx
+++ b/cmu/SurePark/SurePark_Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -445,6 +445,18 @@
   </si>
   <si>
     <t>{userEmail:'gildong@lge.com'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displayName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,8 +625,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="B2:F8" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="B2:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="B2:F9" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="B2:F9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="name" dataDxfId="9"/>
     <tableColumn id="2" name="type" dataDxfId="8"/>
@@ -941,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1056,6 +1068,17 @@
       </c>
       <c r="E8" s="3" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>